<commit_message>
ajout pdf, suppression fichier ._. et corrections sur ano had
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RAFAEL ANO 18.xlsx
+++ b/formats/excel/Formats RAFAEL ANO 18.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ANO-ACE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88">
   <si>
     <t>libelle</t>
   </si>
@@ -122,6 +122,162 @@
   </si>
   <si>
     <t>RBNAIS</t>
+  </si>
+  <si>
+    <t>Signature numérique</t>
+  </si>
+  <si>
+    <t>SIGNATURENUM</t>
+  </si>
+  <si>
+    <t>N° FINESS LAMDA fusion</t>
+  </si>
+  <si>
+    <t>NOFINESS_LAMDA</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Montant total du séjour facturé au patient "</t>
+  </si>
+  <si>
+    <t>CRMTTFACPAT</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Rejet AMO "</t>
+  </si>
+  <si>
+    <t>CRREJETAMO</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de facturation AMO "</t>
+  </si>
+  <si>
+    <t>CRDATFACTAMO</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de facturation AMC "</t>
+  </si>
+  <si>
+    <t>CRDATFACTAMC</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de facturation patient "</t>
+  </si>
+  <si>
+    <t>CRDATFACTPAT</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de paiement AMO "</t>
+  </si>
+  <si>
+    <t>CRDATPAIAMO</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de paiement AMC "</t>
+  </si>
+  <si>
+    <t>CRDATPAIAMC</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Date de paiement patient "</t>
+  </si>
+  <si>
+    <t>CRDATPAIPAT</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Statut FT AMO "</t>
+  </si>
+  <si>
+    <t>CRSTATFTAMO</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Statut FT AMC "</t>
+  </si>
+  <si>
+    <t>CRSTATFTAMC</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Statut FT patient "</t>
+  </si>
+  <si>
+    <t>CRSTATFTPAT</t>
+  </si>
+  <si>
+    <t>Code retour contrôle " Pays d’assurance social "</t>
+  </si>
+  <si>
+    <t>CRPAYSPAT</t>
+  </si>
+  <si>
+    <t>Montant total du séjour facturé au patient</t>
+  </si>
+  <si>
+    <t>MTTFACPAT</t>
+  </si>
+  <si>
+    <t>Rejet AMO</t>
+  </si>
+  <si>
+    <t>REJETAMO</t>
+  </si>
+  <si>
+    <t>Date de facturation AMO</t>
+  </si>
+  <si>
+    <t>DATFACTAMO</t>
+  </si>
+  <si>
+    <t>Date de facturation AMC</t>
+  </si>
+  <si>
+    <t>DATFACTAMC</t>
+  </si>
+  <si>
+    <t>Date de facturation patient</t>
+  </si>
+  <si>
+    <t>DATFACTPAT</t>
+  </si>
+  <si>
+    <t>Date de paiement AMO</t>
+  </si>
+  <si>
+    <t>DATPAIAMO</t>
+  </si>
+  <si>
+    <t>Date de paiement AMC</t>
+  </si>
+  <si>
+    <t>DATPAIAMC</t>
+  </si>
+  <si>
+    <t>Date de paiement patient</t>
+  </si>
+  <si>
+    <t>DATPAIPAT</t>
+  </si>
+  <si>
+    <t>Statut FT AMO</t>
+  </si>
+  <si>
+    <t>STATFTAMO</t>
+  </si>
+  <si>
+    <t>Statut FT AMC</t>
+  </si>
+  <si>
+    <t>STATFTAMC</t>
+  </si>
+  <si>
+    <t>Statut FT patient</t>
+  </si>
+  <si>
+    <t>STATFTPAT</t>
+  </si>
+  <si>
+    <t>Pays d’assurance social</t>
+  </si>
+  <si>
+    <t>PAYSPAT</t>
   </si>
 </sst>
 </file>
@@ -130,11 +286,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +306,37 @@
       <sz val="8"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -167,6 +354,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -176,17 +370,25 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -207,14 +409,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,7 +446,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,32 +467,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,30 +483,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,61 +505,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,31 +679,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,85 +691,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,6 +744,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -575,30 +794,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -616,163 +811,161 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,6 +982,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -798,6 +1010,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,15 +1357,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="55.2833333333333" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1166,7 +1382,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1186,7 +1402,7 @@
       <c r="D2" s="2">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="14" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1206,7 +1422,7 @@
       <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1226,7 +1442,7 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1246,7 +1462,7 @@
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1266,7 +1482,7 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1286,7 +1502,7 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1306,7 +1522,7 @@
       <c r="D8" s="2">
         <v>17</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1326,7 +1542,7 @@
       <c r="D9" s="2">
         <v>5</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1346,29 +1562,29 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" ht="24" spans="1:6">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" ref="B11:B15" si="0">C10+1</f>
+        <f t="shared" ref="B11:B41" si="0">C10+1</f>
         <v>45</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" ref="C11:C15" si="1">B11+D11-1</f>
+        <f t="shared" ref="C11:C41" si="1">B11+D11-1</f>
         <v>61</v>
       </c>
       <c r="D11" s="4">
         <v>17</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1390,7 +1606,7 @@
       <c r="D12" s="5">
         <v>8</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1412,7 +1628,7 @@
       <c r="D13" s="5">
         <v>8</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1434,7 +1650,7 @@
       <c r="D14" s="5">
         <v>3</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1456,10 +1672,582 @@
       <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="D16" s="7">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="7">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="D17" s="7">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" ht="15" spans="1:6">
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:6">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="9">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:6">
+      <c r="A20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="9">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:6">
+      <c r="A21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="9">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:6">
+      <c r="A22" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="9">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:6">
+      <c r="A23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="9">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="C23" s="9">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:6">
+      <c r="A24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="9">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:6">
+      <c r="A25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="9">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="C25" s="9">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="D25" s="10">
+        <v>1</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:6">
+      <c r="A26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="9">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="C26" s="9">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="D26" s="10">
+        <v>1</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" ht="15" spans="1:6">
+      <c r="A27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="9">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="1:6">
+      <c r="A28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="9">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="C28" s="9">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:6">
+      <c r="A29" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="9">
+        <f t="shared" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="C29" s="9">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" ht="15" spans="1:6">
+      <c r="A30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="9">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="1"/>
+        <v>142</v>
+      </c>
+      <c r="D30" s="12">
+        <v>8</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" ht="15" spans="1:6">
+      <c r="A31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="9">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="C31" s="9">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="D31" s="12">
+        <v>1</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" ht="15" spans="1:6">
+      <c r="A32" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="9">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="C32" s="9">
+        <f t="shared" si="1"/>
+        <v>151</v>
+      </c>
+      <c r="D32" s="12">
+        <v>8</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" ht="15" spans="1:6">
+      <c r="A33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="9">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="C33" s="9">
+        <f t="shared" si="1"/>
+        <v>159</v>
+      </c>
+      <c r="D33" s="12">
+        <v>8</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" ht="15" spans="1:6">
+      <c r="A34" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="9">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="C34" s="9">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="D34" s="12">
+        <v>8</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" ht="15" spans="1:6">
+      <c r="A35" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="9">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="C35" s="9">
+        <f t="shared" si="1"/>
+        <v>175</v>
+      </c>
+      <c r="D35" s="12">
+        <v>8</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" ht="15" spans="1:6">
+      <c r="A36" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="9">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="C36" s="9">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="D36" s="12">
+        <v>8</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" ht="15" spans="1:6">
+      <c r="A37" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="9">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="C37" s="9">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="D37" s="12">
+        <v>8</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" ht="15" spans="1:6">
+      <c r="A38" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="9">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="D38" s="12">
+        <v>1</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" ht="15" spans="1:6">
+      <c r="A39" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="9">
+        <f t="shared" si="0"/>
+        <v>193</v>
+      </c>
+      <c r="C39" s="9">
+        <f t="shared" si="1"/>
+        <v>193</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" ht="15" spans="1:6">
+      <c r="A40" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="9">
+        <f t="shared" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="C40" s="9">
+        <f t="shared" si="1"/>
+        <v>194</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" ht="15" spans="1:6">
+      <c r="A41" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="9">
+        <f t="shared" si="0"/>
+        <v>195</v>
+      </c>
+      <c r="C41" s="9">
+        <f t="shared" si="1"/>
+        <v>197</v>
+      </c>
+      <c r="D41" s="12">
+        <v>3</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>